<commit_message>
counter testing in progress. tc 0, 1, 2, 3, 4, 10 completed.
</commit_message>
<xml_diff>
--- a/soberano/test_cases/responsibilities_test_cases_enriched.xlsx
+++ b/soberano/test_cases/responsibilities_test_cases_enriched.xlsx
@@ -305,10 +305,10 @@
   </sheetPr>
   <dimension ref="A1:N34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B13" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
-      <selection pane="topRight" activeCell="E24" activeCellId="0" sqref="E24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B16" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+      <selection pane="topRight" activeCell="A26" activeCellId="0" sqref="26:26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
product category check recording test completed
</commit_message>
<xml_diff>
--- a/soberano/test_cases/responsibilities_test_cases_enriched.xlsx
+++ b/soberano/test_cases/responsibilities_test_cases_enriched.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="53">
   <si>
     <t xml:space="preserve">User</t>
   </si>
@@ -164,6 +164,9 @@
   </si>
   <si>
     <t xml:space="preserve">user20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user21</t>
   </si>
   <si>
     <t xml:space="preserve">workshop1Worker</t>
@@ -315,12 +318,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N38"/>
+  <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="K22" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
-      <selection pane="topRight" activeCell="N43" activeCellId="0" sqref="N43"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="0" topLeftCell="B16" activePane="topRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
+      <selection pane="topRight" activeCell="N34" activeCellId="0" sqref="N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1791,48 +1794,48 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B34" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="E34" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="F34" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="G34" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H34" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="I34" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="J34" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="K34" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="L34" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="M34" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="N34" s="0" t="s">
-        <v>15</v>
+      <c r="B34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1858,10 +1861,10 @@
         <v>15</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J35" s="0" t="s">
         <v>15</v>
@@ -1880,28 +1883,72 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="2" t="s">
+      <c r="A36" s="0" t="s">
         <v>50</v>
       </c>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
-    </row>
-    <row r="38" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="s">
+      <c r="B36" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="C36" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="E36" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="F36" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="H36" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I36" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="J36" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K36" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="L36" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="M36" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="N36" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2" t="s">
         <v>51</v>
+      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="2"/>
+      <c r="L37" s="2"/>
+      <c r="M37" s="2"/>
+      <c r="N37" s="2"/>
+    </row>
+    <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
warehouse disabling in progress
</commit_message>
<xml_diff>
--- a/soberano/test_cases/responsibilities_test_cases_enriched.xlsx
+++ b/soberano/test_cases/responsibilities_test_cases_enriched.xlsx
@@ -320,10 +320,12 @@
   </sheetPr>
   <dimension ref="A1:N39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="0" topLeftCell="B16" activePane="topRight" state="frozen"/>
-      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16"/>
-      <selection pane="topRight" activeCell="N34" activeCellId="0" sqref="N34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="J20" activePane="bottomRight" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+      <selection pane="bottomRight" activeCell="K39" activeCellId="0" sqref="K39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
cost center recording testing completed
</commit_message>
<xml_diff>
--- a/soberano/test_cases/responsibilities_test_cases_enriched.xlsx
+++ b/soberano/test_cases/responsibilities_test_cases_enriched.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="54">
   <si>
     <t xml:space="preserve">User</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t xml:space="preserve">14_SystemAdmin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15_Technologist</t>
   </si>
   <si>
     <t xml:space="preserve">accounter</t>
@@ -318,17 +321,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N39"/>
+  <dimension ref="A1:O1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="M14" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
-      <selection pane="bottomRight" activeCell="K39" activeCellId="0" sqref="K39"/>
+      <selection pane="topRight" activeCell="M1" activeCellId="0" sqref="M1"/>
+      <selection pane="bottomLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+      <selection pane="bottomRight" activeCell="P34" activeCellId="0" sqref="P34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.05"/>
@@ -342,9 +345,10 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="23.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="22.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="14.7"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -387,1554 +391,1662 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+      <c r="O2" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+      <c r="O4" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+      <c r="O5" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N6" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+      <c r="O6" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N7" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+      <c r="O7" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N8" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+      <c r="O8" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N9" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+      <c r="O9" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N10" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+      <c r="O10" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N11" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+      <c r="O11" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N12" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+      <c r="O12" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M13" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N13" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+      <c r="O13" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N14" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+      <c r="O14" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N15" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+      <c r="O15" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M16" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N16" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+      <c r="O16" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L17" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M17" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N17" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+      <c r="O17" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M18" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N18" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+      <c r="O18" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L19" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M19" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N19" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+      <c r="O19" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L20" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M20" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N20" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+      <c r="O20" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L21" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M21" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N21" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+      <c r="O21" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L22" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M22" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N22" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+      <c r="O22" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L23" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M23" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N23" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+      <c r="O23" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L24" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M24" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N24" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+      <c r="O24" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L25" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M25" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N25" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+      <c r="O25" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K26" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L26" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M26" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N26" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+      <c r="O26" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K27" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L27" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M27" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N27" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+      <c r="O27" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K28" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L28" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M28" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+      <c r="O28" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K29" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L29" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M29" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N29" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="O29" s="0" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="O30" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="O31" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="O32" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="O33" s="0" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>17</v>
+      </c>
+      <c r="O34" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J35" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K35" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L35" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M35" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N35" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+      <c r="O35" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="K36" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L36" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="M36" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="N36" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+      <c r="O36" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -1947,12 +2059,16 @@
       <c r="L37" s="2"/>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
+      <c r="O37" s="0" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>52</v>
-      </c>
-    </row>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
order recording completed. order management form coding in progress.
</commit_message>
<xml_diff>
--- a/soberano/test_cases/responsibilities_test_cases_enriched.xlsx
+++ b/soberano/test_cases/responsibilities_test_cases_enriched.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="56">
   <si>
     <t xml:space="preserve">User</t>
   </si>
@@ -67,6 +67,9 @@
     <t xml:space="preserve">15_Technologist</t>
   </si>
   <si>
+    <t xml:space="preserve">16_ManagerAssitant</t>
+  </si>
+  <si>
     <t xml:space="preserve">accounter</t>
   </si>
   <si>
@@ -170,6 +173,9 @@
   </si>
   <si>
     <t xml:space="preserve">user21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">user22</t>
   </si>
   <si>
     <t xml:space="preserve">workshop1Worker</t>
@@ -321,14 +327,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O39"/>
+  <dimension ref="A1:P40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="N23" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="N40" activeCellId="0" sqref="N40"/>
+      <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="bottomLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+      <selection pane="bottomRight" activeCell="R29" activeCellId="0" sqref="R29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -345,7 +351,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="23.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="22.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -394,1678 +401,1839 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="P6" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N8" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N9" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N10" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="P10" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N11" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="P11" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N12" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M13" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N13" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N14" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P14" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N15" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M16" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N16" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P16" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L17" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M17" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N17" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M18" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N18" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P18" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L19" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M19" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N19" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L20" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M20" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N20" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P20" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L21" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M21" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N21" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L22" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M22" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N22" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P22" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L23" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M23" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N23" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L24" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M24" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N24" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O24" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P24" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L25" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M25" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N25" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K26" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L26" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M26" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N26" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O26" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P26" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K27" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L27" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M27" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N27" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K28" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L28" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M28" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P28" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K29" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L29" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M29" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="P29" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O30" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P30" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="P31" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O32" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P32" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O33" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="P33" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="P34" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E35" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="F35" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="G35" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="H35" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="I35" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="J35" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="K35" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="L35" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="M35" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="N35" s="0" t="s">
-        <v>16</v>
+      <c r="A35" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N35" s="2" t="s">
+        <v>17</v>
       </c>
       <c r="O35" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="P35" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="I36" s="0" t="s">
         <v>17</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K36" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L36" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M36" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="N36" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="O36" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
+      </c>
+      <c r="P36" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B37" s="2"/>
-      <c r="C37" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D37" s="2"/>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
+      <c r="A37" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="E37" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F37" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="H37" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I37" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J37" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="K37" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="L37" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="M37" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="N37" s="0" t="s">
+        <v>17</v>
+      </c>
       <c r="O37" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="P37" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2" t="s">
         <v>53</v>
+      </c>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P38" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
order and receivable collecting completed.
</commit_message>
<xml_diff>
--- a/soberano/test_cases/responsibilities_test_cases_enriched.xlsx
+++ b/soberano/test_cases/responsibilities_test_cases_enriched.xlsx
@@ -330,11 +330,11 @@
   <dimension ref="A1:P40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="N23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
-      <selection pane="bottomRight" activeCell="R29" activeCellId="0" sqref="R29"/>
+      <selection pane="bottomRight" activeCell="B33" activeCellId="0" sqref="33:33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
testing order reopening in progress. problems with corresponding inventory recalculation. buggy.
</commit_message>
<xml_diff>
--- a/soberano/test_cases/responsibilities_test_cases_enriched.xlsx
+++ b/soberano/test_cases/responsibilities_test_cases_enriched.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="57">
   <si>
     <t xml:space="preserve">User</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t xml:space="preserve">16_ManagerAssitant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18_Reopener</t>
   </si>
   <si>
     <t xml:space="preserve">accounter</t>
@@ -327,14 +330,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P40"/>
+  <dimension ref="A1:Q40"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="M26" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
-      <selection pane="bottomRight" activeCell="B33" activeCellId="0" sqref="33:33"/>
+      <selection pane="topRight" activeCell="M1" activeCellId="0" sqref="M1"/>
+      <selection pane="bottomLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
+      <selection pane="bottomRight" activeCell="O35" activeCellId="0" sqref="35:35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -353,6 +356,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="17.97"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -404,1814 +408,1925 @@
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N6" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N9" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N10" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N11" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N12" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M13" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N13" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N14" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N15" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M16" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N16" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O16" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L17" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M17" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N17" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M18" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N18" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L19" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M19" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N19" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L20" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M20" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N20" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L21" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M21" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N21" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L22" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M22" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N22" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L23" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M23" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N23" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L24" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M24" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N24" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="Q24" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L25" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M25" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N25" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K26" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L26" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M26" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N26" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J27" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K27" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L27" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M27" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N27" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="Q27" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J28" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="K28" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L28" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M28" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N28" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P28" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="Q28" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K29" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="L29" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="M29" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N29" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="Q29" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P30" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="Q30" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="Q31" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P32" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="Q32" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O33" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="Q33" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P34" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="Q34" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O35" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
+      </c>
+      <c r="Q35" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K36" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L36" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M36" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N36" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O36" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P36" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="Q36" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J37" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K37" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L37" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M37" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N37" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="O37" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P37" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="Q37" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -2225,15 +2340,18 @@
       <c r="M38" s="2"/>
       <c r="N38" s="2"/>
       <c r="O38" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="P38" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="Q38" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
multiple printing of an order's process run output allocations is now prevented. now, they are printed once. code completed.
translations of order and process run histories were corrected. it was
just to insert chr(13) between every pair of tokens to translate. if
not, regex coming with java 8 wouldn't have processed properly.

correction allowing quantities equal to zero in process (and process
runs) inputs and outputs.
</commit_message>
<xml_diff>
--- a/soberano/test_cases/responsibilities_test_cases_enriched.xlsx
+++ b/soberano/test_cases/responsibilities_test_cases_enriched.xlsx
@@ -67,7 +67,7 @@
     <t xml:space="preserve">15_Technologist</t>
   </si>
   <si>
-    <t xml:space="preserve">16_ManagerAssitant</t>
+    <t xml:space="preserve">16_ManagerAssistant</t>
   </si>
   <si>
     <t xml:space="preserve">18_Reopener</t>
@@ -337,7 +337,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="M1" activeCellId="0" sqref="M1"/>
       <selection pane="bottomLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
-      <selection pane="bottomRight" activeCell="O35" activeCellId="0" sqref="35:35"/>
+      <selection pane="bottomRight" activeCell="P1" activeCellId="0" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -356,7 +356,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="17.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="12.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="20.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="17.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="17.98"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>